<commit_message>
update environmental data: Lightstation data PDO data Site slope and area
</commit_message>
<xml_diff>
--- a/Data/Site maps + topography/slope_aspect_summaries.xlsx
+++ b/Data/Site maps + topography/slope_aspect_summaries.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20376"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mawha\Dropbox\Martone Lab\martone_calvert\Data\Site maps + topography\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623C6D34-6310-4A6A-AEEF-BFD69E8A675D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C8C327-5E46-409D-9F7E-0CB8C31B3774}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{C98054CC-C0AF-4475-9F0B-6B319F60286B}"/>
   </bookViews>
@@ -17,25 +17,20 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$E$13</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="16">
   <si>
     <t>site</t>
   </si>
@@ -68,6 +63,21 @@
   </si>
   <si>
     <t>fifth_beach</t>
+  </si>
+  <si>
+    <t>compass</t>
+  </si>
+  <si>
+    <t>SbW</t>
+  </si>
+  <si>
+    <t>SSW</t>
+  </si>
+  <si>
+    <t>shallowest</t>
+  </si>
+  <si>
+    <t>steepest</t>
   </si>
 </sst>
 </file>
@@ -75,7 +85,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -106,12 +116,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,19 +437,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A28AEA3-17EC-4ABC-8AEF-5F765AB6A6ED}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6328125" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" customWidth="1"/>
+    <col min="4" max="4" width="17.54296875" customWidth="1"/>
+    <col min="5" max="5" width="17.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -454,44 +467,53 @@
       <c r="E1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>15.463490999999999</v>
-      </c>
-      <c r="E2">
-        <v>14.466937</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D2" s="3">
+        <v>188.397111</v>
+      </c>
+      <c r="E2" s="3">
+        <v>108.72356600000001</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3">
-        <v>19.897329507575758</v>
-      </c>
-      <c r="E3">
-        <v>17.075900681758931</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>223.6687</v>
+      </c>
+      <c r="E3" s="3">
+        <v>88.872550000000004</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -499,31 +521,37 @@
       <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="D4">
-        <v>188.397111</v>
-      </c>
-      <c r="E4">
-        <v>108.72356600000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D4" s="3">
+        <v>197.78352100000001</v>
+      </c>
+      <c r="E4" s="3">
+        <v>101.77290000000001</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5">
-        <v>180.21042293939399</v>
-      </c>
-      <c r="E5">
-        <v>112.335959666668</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>15.463490999999999</v>
+      </c>
+      <c r="E5" s="3">
+        <v>14.466937</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -533,48 +561,51 @@
       <c r="C6" t="s">
         <v>0</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>25.318570000000001</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <v>18.491299999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7">
-        <v>25.691423702702707</v>
-      </c>
-      <c r="E7">
-        <v>18.406734123936062</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>32.045243999999997</v>
+      </c>
+      <c r="E7" s="3">
+        <v>20.283567999999999</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>223.6687</v>
-      </c>
-      <c r="E8">
-        <v>88.872550000000004</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="D8" s="3">
+        <v>180.21042293939399</v>
+      </c>
+      <c r="E8" s="3">
+        <v>112.335959666668</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -584,33 +615,33 @@
       <c r="C9" t="s">
         <v>9</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>240.98670067567556</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <v>79.199683305384013</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>32.045243999999997</v>
-      </c>
-      <c r="E10">
-        <v>20.283567999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="D10" s="3">
+        <v>186.59902491463421</v>
+      </c>
+      <c r="E10" s="3">
+        <v>102.16389622073926</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -618,49 +649,146 @@
       <c r="C11" t="s">
         <v>9</v>
       </c>
-      <c r="D11">
-        <v>26.208088604938272</v>
-      </c>
-      <c r="E11">
-        <v>20.270319430644154</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D11" s="3">
+        <v>19.897329507575758</v>
+      </c>
+      <c r="E11" s="3">
+        <v>17.075900681758931</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>197.78352100000001</v>
-      </c>
-      <c r="E12">
-        <v>101.77290000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="D12" s="3">
+        <v>25.691423702702707</v>
+      </c>
+      <c r="E12" s="3">
+        <v>18.406734123936062</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
       </c>
-      <c r="D13">
-        <v>186.59902491463421</v>
-      </c>
-      <c r="E13">
-        <v>102.16389622073926</v>
+      <c r="D13" s="3">
+        <v>26.208088604938272</v>
+      </c>
+      <c r="E13" s="3">
+        <v>20.270319430644154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="3">
+        <f>AVERAGE(D2,D8)</f>
+        <v>184.30376696969699</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="3">
+        <f>AVERAGE(D3,D9)</f>
+        <v>232.32770033783777</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" ref="D16:D19" si="0">AVERAGE(D4,D10)</f>
+        <v>192.1912729573171</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="3">
+        <f>AVERAGE(D5,D11)</f>
+        <v>17.68041025378788</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="0"/>
+        <v>25.504996851351354</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="0"/>
+        <v>29.126666302469133</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E13" xr:uid="{2B6B94C0-5398-4429-86D5-4CDB66539310}">
+    <sortState ref="A2:E13">
+      <sortCondition ref="C2:C13"/>
+      <sortCondition ref="B2:B13"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -673,14 +801,14 @@
       <selection sqref="A1:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.77734375" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -697,7 +825,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -714,7 +842,7 @@
         <v>14.466937</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -731,7 +859,7 @@
         <v>17.075900681758931</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -748,7 +876,7 @@
         <v>108.72356600000001</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -765,7 +893,7 @@
         <v>112.335959666668</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -782,7 +910,7 @@
         <v>18.491299999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -799,7 +927,7 @@
         <v>18.406734123936062</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -816,7 +944,7 @@
         <v>88.872550000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -833,7 +961,7 @@
         <v>79.199683305384013</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -850,7 +978,7 @@
         <v>20.283567999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -867,7 +995,7 @@
         <v>20.270319430644154</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -884,7 +1012,7 @@
         <v>101.77290000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>

</xml_diff>